<commit_message>
Add changes to general page
</commit_message>
<xml_diff>
--- a/files/beef.xlsx
+++ b/files/beef.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Desktop\Adalab\Pair-Programming\Modulo-4\promog-modulo4-sprint2-pairprogramming-marina_escobar-isabel_correal\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D148097B-261C-41B5-BF20-0DEC004B24CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B206A60-9B55-4A9A-BAFF-9A31D1B7B833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15345" xr2:uid="{BE06563D-F197-4548-8C70-5C4CDDF48CD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{BE06563D-F197-4548-8C70-5C4CDDF48CD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$63</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="100">
   <si>
     <t>Source</t>
   </si>
@@ -252,28 +252,91 @@
     <t>https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680</t>
   </si>
   <si>
-    <t>https://hips.hearstapps.com/hmg-prod/images/joe-jonas-pelo-2021-1628003622.jpg</t>
-  </si>
-  <si>
-    <t>https://graziamagazine.com/mx/wp-content/uploads/sites/13/2018/01/blake-lively-cambia-look-nueva-pelicula-the-rythm-section-destacada.jpg</t>
-  </si>
-  <si>
-    <t>https://media.revistavanityfair.es/photos/60e849cefc86fee32f97d0b4/master/w_1600%2Cc_limit/48924.jpg</t>
-  </si>
-  <si>
-    <t>https://media.vogue.mx/photos/64504ef0485b8e1becf736b5/2:3/w_2560%2Cc_limit/Screen%2520Shot%25202023-05-01%2520at%25207.21.22%2520PM.png</t>
-  </si>
-  <si>
-    <t>https://upload.wikimedia.org/wikipedia/commons/2/2c/Katy_Perry_for_Vogue_Magazine%2C_2023.png</t>
-  </si>
-  <si>
-    <t>https://media-cldnry.s-nbcnews.com/image/upload/t_fit-1500w,f_auto,q_auto:best/rockcms/2023-12/lena-dunham-jp-231211-0fb74b.jpg</t>
-  </si>
-  <si>
-    <t>https://images.ecestaticos.com/BdqKvazRWczn2CaY35AeT-7Qw4k=/0x0:0x0/1200x900/filters:fill(white):format(jpg)/f.elconfidencial.com%2Foriginal%2Fa15%2Fa45%2Fc36%2Fa15a45c369f7638442cfaeac8f1611fc.jpg</t>
-  </si>
-  <si>
-    <t>https://hips.hearstapps.com/hmg-prod/images/singer-and-actress-selena-gomez-arrives-for-the-mtv-video-news-photo-1694562661.jpg</t>
+    <t>https://www.thesun.ie/wp-content/uploads/sites/3/2019/06/SC-Joe-Jonas-Off-Plat-copy.jpg?strip=all&amp;quality=100&amp;w=1080&amp;h=1080&amp;crop=1</t>
+  </si>
+  <si>
+    <t>https://cdn.britannica.com/16/141316-050-21139A4F/John-Mayer-2008.jpg</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn3.gstatic.com/images?q=tbn:ANd9GcRHaTNjXAXSrNybs6Y2jumnwHo8J8SnPentvlIdKV_ykSI1cC28</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn3.gstatic.com/images?q=tbn:ANd9GcR9_AFzGUC8Rr6PO5HMkanKO3H8ZHhM8NY9vOKaXe7SvekeNyE-</t>
+  </si>
+  <si>
+    <t>https://encrypted-tbn3.gstatic.com/images?q=tbn:ANd9GcQoEynv5e958e8xL9EOSHNhLH3zq29bZBjo3JeRbNx-ssgaJmtt</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/WC6Z6eJ.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/YDAjwoX.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/GmNTWb6.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/bjDYJM5.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/Nu5ux0K.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/xBTidI0.jpeg</t>
+  </si>
+  <si>
+    <t>https://upload.wikimedia.org/wikipedia/commons/thumb/2/27/Lorde_%282022%29_%28cropped%29.jpg/640px-Lorde_%282022%29_%28cropped%29.jpg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/1t2IPVp.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/PONfKOP.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/QJxTixy.png</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/bVXYq5p.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/U25Fetn.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/svCAQfd.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/ArmNi0c.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/T2yfGfd.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/31tF8gh.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/CmJcTt0.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/bBLTGil.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/JmOCr7B.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IGBUcMC.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/e3weU0p.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/SfRDNYu.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/3WPTfSk.jpeg</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/11c15yD.jpeg</t>
   </si>
 </sst>
 </file>
@@ -303,18 +366,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -332,8 +389,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,11 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C83D10-D6CD-43BE-91E0-25A15ABA6B36}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,7 +757,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -726,14 +782,14 @@
       <c r="H2">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -755,11 +811,11 @@
       <c r="H3">
         <v>5</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>78</v>
+      <c r="I3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -784,11 +840,14 @@
       <c r="H4">
         <v>5</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -810,14 +869,14 @@
       <c r="H5">
         <v>5</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -842,11 +901,11 @@
       <c r="H6">
         <v>5</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>73</v>
+      <c r="I6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -871,11 +930,14 @@
       <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -897,14 +959,14 @@
       <c r="H8">
         <v>5</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -926,11 +988,11 @@
       <c r="H9">
         <v>5</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>73</v>
+      <c r="I9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -955,8 +1017,11 @@
       <c r="H10">
         <v>5</v>
       </c>
-      <c r="I10" s="2" t="s">
-        <v>70</v>
+      <c r="I10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -964,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>2011</v>
@@ -973,7 +1038,7 @@
         <v>26</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G11">
         <v>10</v>
@@ -981,25 +1046,28 @@
       <c r="H11">
         <v>5</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>70</v>
+      <c r="I11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C12">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D12" t="s">
         <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G12">
         <v>10</v>
@@ -1007,16 +1075,19 @@
       <c r="H12">
         <v>5</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>2012</v>
@@ -1025,7 +1096,7 @@
         <v>26</v>
       </c>
       <c r="E13" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="G13">
         <v>10</v>
@@ -1033,11 +1104,11 @@
       <c r="H13">
         <v>5</v>
       </c>
-      <c r="I13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>75</v>
+      <c r="I13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1045,7 +1116,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C14">
         <v>2012</v>
@@ -1054,7 +1125,7 @@
         <v>26</v>
       </c>
       <c r="E14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G14">
         <v>10</v>
@@ -1062,16 +1133,19 @@
       <c r="H14">
         <v>5</v>
       </c>
-      <c r="I14" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>2012</v>
@@ -1080,7 +1154,7 @@
         <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G15">
         <v>10</v>
@@ -1088,11 +1162,11 @@
       <c r="H15">
         <v>5</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>74</v>
+      <c r="I15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1100,7 +1174,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <v>2012</v>
@@ -1109,7 +1183,7 @@
         <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G16">
         <v>10</v>
@@ -1117,8 +1191,11 @@
       <c r="H16">
         <v>5</v>
       </c>
-      <c r="I16" s="2" t="s">
-        <v>70</v>
+      <c r="I16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -1126,7 +1203,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17">
         <v>2012</v>
@@ -1135,7 +1212,7 @@
         <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G17">
         <v>10</v>
@@ -1143,8 +1220,11 @@
       <c r="H17">
         <v>5</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>70</v>
+      <c r="I17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -1155,13 +1235,13 @@
         <v>28</v>
       </c>
       <c r="C18">
-        <v>2013</v>
-      </c>
-      <c r="D18">
-        <v>1989</v>
+        <v>2012</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="G18">
         <v>10</v>
@@ -1169,8 +1249,11 @@
       <c r="H18">
         <v>5</v>
       </c>
-      <c r="I18" s="2" t="s">
-        <v>70</v>
+      <c r="I18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -1178,7 +1261,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>2013</v>
@@ -1187,7 +1270,10 @@
         <v>1989</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
       </c>
       <c r="G19">
         <v>10</v>
@@ -1195,16 +1281,19 @@
       <c r="H19">
         <v>5</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>70</v>
+      <c r="I19" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>2013</v>
@@ -1213,7 +1302,7 @@
         <v>1989</v>
       </c>
       <c r="E20" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G20">
         <v>10</v>
@@ -1221,16 +1310,19 @@
       <c r="H20">
         <v>5</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C21">
         <v>2013</v>
@@ -1247,8 +1339,11 @@
       <c r="H21">
         <v>5</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>70</v>
+      <c r="I21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -1256,7 +1351,7 @@
         <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>2013</v>
@@ -1265,7 +1360,7 @@
         <v>1989</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G22">
         <v>10</v>
@@ -1273,16 +1368,19 @@
       <c r="H22">
         <v>5</v>
       </c>
-      <c r="I22" s="2" t="s">
-        <v>70</v>
+      <c r="I22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C23">
         <v>2013</v>
@@ -1291,7 +1389,7 @@
         <v>1989</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G23">
         <v>10</v>
@@ -1299,8 +1397,11 @@
       <c r="H23">
         <v>5</v>
       </c>
-      <c r="I23" s="2" t="s">
-        <v>73</v>
+      <c r="I23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1308,10 +1409,10 @@
         <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C24">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D24">
         <v>1989</v>
@@ -1325,28 +1426,28 @@
       <c r="H24">
         <v>5</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C25">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D25">
         <v>1989</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G25">
         <v>10</v>
@@ -1354,22 +1455,22 @@
       <c r="H25">
         <v>5</v>
       </c>
-      <c r="I25" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C26">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D26">
         <v>1989</v>
@@ -1383,28 +1484,28 @@
       <c r="H26">
         <v>5</v>
       </c>
-      <c r="I26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>76</v>
+      <c r="I26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C27">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D27">
         <v>1989</v>
       </c>
       <c r="E27" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="G27">
         <v>10</v>
@@ -1412,25 +1513,28 @@
       <c r="H27">
         <v>5</v>
       </c>
-      <c r="I27" s="2" t="s">
-        <v>76</v>
+      <c r="I27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C28">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D28">
         <v>1989</v>
       </c>
       <c r="E28" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="G28">
         <v>10</v>
@@ -1438,16 +1542,19 @@
       <c r="H28">
         <v>5</v>
       </c>
-      <c r="I28" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C29">
         <v>2014</v>
@@ -1456,7 +1563,7 @@
         <v>1989</v>
       </c>
       <c r="E29" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="G29">
         <v>10</v>
@@ -1464,11 +1571,11 @@
       <c r="H29">
         <v>5</v>
       </c>
-      <c r="I29" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>75</v>
+      <c r="I29" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
@@ -1476,19 +1583,19 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C30">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D30">
         <v>1989</v>
       </c>
       <c r="E30" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G30">
         <v>10</v>
@@ -1496,19 +1603,22 @@
       <c r="H30">
         <v>5</v>
       </c>
-      <c r="I30" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C31">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D31">
         <v>1989</v>
@@ -1516,40 +1626,34 @@
       <c r="E31" t="s">
         <v>19</v>
       </c>
-      <c r="F31" t="s">
-        <v>39</v>
-      </c>
       <c r="G31">
         <v>10</v>
       </c>
       <c r="H31">
         <v>5</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D32">
         <v>1989</v>
       </c>
       <c r="E32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="G32">
         <v>10</v>
@@ -1557,22 +1661,22 @@
       <c r="H32">
         <v>5</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>77</v>
+      <c r="I32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C33">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D33">
         <v>1989</v>
@@ -1580,95 +1684,98 @@
       <c r="E33" t="s">
         <v>37</v>
       </c>
-      <c r="F33" t="s">
-        <v>39</v>
-      </c>
       <c r="G33">
         <v>10</v>
       </c>
       <c r="H33">
         <v>5</v>
       </c>
-      <c r="I33" s="2" t="s">
-        <v>77</v>
+      <c r="I33" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C34">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D34">
         <v>1989</v>
       </c>
       <c r="E34" t="s">
+        <v>31</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+      <c r="H34">
+        <v>5</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>2015</v>
+      </c>
+      <c r="D35">
+        <v>1989</v>
+      </c>
+      <c r="E35" t="s">
         <v>50</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F35" t="s">
         <v>39</v>
       </c>
-      <c r="G34">
-        <v>10</v>
-      </c>
-      <c r="H34">
-        <v>5</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>22</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35">
-        <v>2016</v>
-      </c>
-      <c r="D35" t="s">
-        <v>44</v>
-      </c>
-      <c r="E35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" t="s">
-        <v>46</v>
-      </c>
       <c r="G35">
         <v>10</v>
       </c>
       <c r="H35">
         <v>5</v>
       </c>
-      <c r="I35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>73</v>
+      <c r="I35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C36">
-        <v>2016</v>
-      </c>
-      <c r="D36" t="s">
-        <v>44</v>
+        <v>2015</v>
+      </c>
+      <c r="D36">
+        <v>1989</v>
       </c>
       <c r="E36" t="s">
-        <v>45</v>
+        <v>19</v>
+      </c>
+      <c r="F36" t="s">
+        <v>39</v>
       </c>
       <c r="G36">
         <v>10</v>
@@ -1676,25 +1783,31 @@
       <c r="H36">
         <v>5</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="I36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J36" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C37">
-        <v>2016</v>
-      </c>
-      <c r="D37" t="s">
-        <v>44</v>
+        <v>2015</v>
+      </c>
+      <c r="D37">
+        <v>1989</v>
       </c>
       <c r="E37" t="s">
-        <v>13</v>
+        <v>43</v>
+      </c>
+      <c r="F37" t="s">
+        <v>39</v>
       </c>
       <c r="G37">
         <v>10</v>
@@ -1702,28 +1815,31 @@
       <c r="H37">
         <v>5</v>
       </c>
-      <c r="I37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>73</v>
+      <c r="I37" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="C38">
-        <v>2016</v>
-      </c>
-      <c r="D38" t="s">
-        <v>44</v>
+        <v>2015</v>
+      </c>
+      <c r="D38">
+        <v>1989</v>
       </c>
       <c r="E38" t="s">
-        <v>50</v>
+        <v>37</v>
+      </c>
+      <c r="F38" t="s">
+        <v>39</v>
       </c>
       <c r="G38">
         <v>10</v>
@@ -1731,25 +1847,31 @@
       <c r="H38">
         <v>5</v>
       </c>
-      <c r="I38" s="2" t="s">
-        <v>73</v>
+      <c r="I38" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C39">
-        <v>2016</v>
-      </c>
-      <c r="D39" t="s">
-        <v>44</v>
+        <v>2015</v>
+      </c>
+      <c r="D39">
+        <v>1989</v>
       </c>
       <c r="E39" t="s">
-        <v>51</v>
+        <v>50</v>
+      </c>
+      <c r="F39" t="s">
+        <v>39</v>
       </c>
       <c r="G39">
         <v>10</v>
@@ -1757,16 +1879,19 @@
       <c r="H39">
         <v>5</v>
       </c>
-      <c r="I39" s="2" t="s">
-        <v>70</v>
+      <c r="I39" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C40">
         <v>2016</v>
@@ -1775,7 +1900,7 @@
         <v>44</v>
       </c>
       <c r="E40" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="G40">
         <v>10</v>
@@ -1783,16 +1908,19 @@
       <c r="H40">
         <v>5</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J40" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>3</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C41">
         <v>2016</v>
@@ -1801,7 +1929,7 @@
         <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="G41">
         <v>10</v>
@@ -1809,19 +1937,19 @@
       <c r="H41">
         <v>5</v>
       </c>
-      <c r="I41" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J41" s="2" t="s">
-        <v>74</v>
+      <c r="I41" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="C42">
         <v>2016</v>
@@ -1830,7 +1958,10 @@
         <v>44</v>
       </c>
       <c r="E42" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="F42" t="s">
+        <v>46</v>
       </c>
       <c r="G42">
         <v>10</v>
@@ -1838,16 +1969,19 @@
       <c r="H42">
         <v>5</v>
       </c>
-      <c r="I42" s="2" t="s">
-        <v>70</v>
+      <c r="I42" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>2016</v>
@@ -1856,7 +1990,7 @@
         <v>44</v>
       </c>
       <c r="E43" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G43">
         <v>10</v>
@@ -1864,16 +1998,19 @@
       <c r="H43">
         <v>5</v>
       </c>
-      <c r="I43" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I43" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>2016</v>
@@ -1882,10 +2019,7 @@
         <v>44</v>
       </c>
       <c r="E44" t="s">
-        <v>55</v>
-      </c>
-      <c r="F44" t="s">
-        <v>56</v>
+        <v>13</v>
       </c>
       <c r="G44">
         <v>10</v>
@@ -1893,38 +2027,40 @@
       <c r="H44">
         <v>5</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>75</v>
+      <c r="I44" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="1">
-        <v>2017</v>
-      </c>
-      <c r="D45" s="1" t="s">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>2016</v>
+      </c>
+      <c r="D45" t="s">
         <v>44</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" s="1"/>
+      <c r="E45" t="s">
+        <v>50</v>
+      </c>
       <c r="G45">
         <v>10</v>
       </c>
       <c r="H45">
         <v>5</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>76</v>
+      <c r="I45" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
@@ -1932,16 +2068,16 @@
         <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C46">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D46" t="s">
         <v>44</v>
       </c>
       <c r="E46" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G46">
         <v>10</v>
@@ -1949,138 +2085,147 @@
       <c r="H46">
         <v>5</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47">
+        <v>2016</v>
+      </c>
+      <c r="D47" t="s">
+        <v>44</v>
+      </c>
+      <c r="E47" t="s">
+        <v>45</v>
+      </c>
+      <c r="G47">
+        <v>10</v>
+      </c>
+      <c r="H47">
+        <v>5</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" t="s">
         <v>22</v>
       </c>
-      <c r="C47">
-        <v>2018</v>
-      </c>
-      <c r="D47" t="s">
-        <v>58</v>
-      </c>
-      <c r="E47" t="s">
-        <v>52</v>
-      </c>
-      <c r="G47">
-        <v>10</v>
-      </c>
-      <c r="H47">
-        <v>5</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J47" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>3</v>
-      </c>
-      <c r="B48" t="s">
+      <c r="C48">
+        <v>2016</v>
+      </c>
+      <c r="D48" t="s">
+        <v>44</v>
+      </c>
+      <c r="E48" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48">
+        <v>10</v>
+      </c>
+      <c r="H48">
+        <v>5</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49">
+        <v>2016</v>
+      </c>
+      <c r="D49" t="s">
+        <v>44</v>
+      </c>
+      <c r="E49" t="s">
+        <v>54</v>
+      </c>
+      <c r="G49">
+        <v>10</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50">
+        <v>2016</v>
+      </c>
+      <c r="D50" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50">
+        <v>10</v>
+      </c>
+      <c r="H50">
+        <v>5</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" t="s">
         <v>15</v>
       </c>
-      <c r="C48">
-        <v>2018</v>
-      </c>
-      <c r="D48" t="s">
-        <v>58</v>
-      </c>
-      <c r="E48" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48">
-        <v>10</v>
-      </c>
-      <c r="H48">
-        <v>5</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" t="s">
-        <v>47</v>
-      </c>
-      <c r="C49">
-        <v>2019</v>
-      </c>
-      <c r="D49" t="s">
-        <v>58</v>
-      </c>
-      <c r="E49" t="s">
-        <v>13</v>
-      </c>
-      <c r="F49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G49">
-        <v>10</v>
-      </c>
-      <c r="H49">
-        <v>5</v>
-      </c>
-      <c r="I49" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>3</v>
-      </c>
-      <c r="B50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50">
-        <v>2021</v>
-      </c>
-      <c r="D50" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50">
-        <v>10</v>
-      </c>
-      <c r="H50">
-        <v>5</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>3</v>
-      </c>
-      <c r="B51" t="s">
-        <v>62</v>
-      </c>
       <c r="C51">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="D51" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E51" t="s">
-        <v>31</v>
+        <v>55</v>
+      </c>
+      <c r="F51" t="s">
+        <v>56</v>
       </c>
       <c r="G51">
         <v>10</v>
@@ -2088,48 +2233,55 @@
       <c r="H51">
         <v>5</v>
       </c>
-      <c r="I51" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>3</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="I51" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="2">
+        <v>2017</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52">
+        <v>10</v>
+      </c>
+      <c r="H52">
+        <v>5</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" t="s">
         <v>57</v>
       </c>
-      <c r="C52">
-        <v>2023</v>
-      </c>
-      <c r="D52" t="s">
-        <v>63</v>
-      </c>
-      <c r="E52" t="s">
-        <v>54</v>
-      </c>
-      <c r="G52">
-        <v>10</v>
-      </c>
-      <c r="H52">
-        <v>5</v>
-      </c>
-      <c r="I52" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" t="s">
-        <v>64</v>
-      </c>
       <c r="C53">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="D53" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="E53" t="s">
         <v>50</v>
@@ -2140,86 +2292,405 @@
       <c r="H53">
         <v>5</v>
       </c>
-      <c r="I53" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="B54" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54">
+        <v>2018</v>
+      </c>
+      <c r="D54" t="s">
+        <v>58</v>
+      </c>
+      <c r="E54" t="s">
+        <v>45</v>
+      </c>
+      <c r="G54">
+        <v>10</v>
+      </c>
+      <c r="H54">
+        <v>5</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" t="s">
+        <v>22</v>
+      </c>
+      <c r="C55">
+        <v>2018</v>
+      </c>
+      <c r="D55" t="s">
+        <v>58</v>
+      </c>
+      <c r="E55" t="s">
+        <v>52</v>
+      </c>
+      <c r="G55">
+        <v>10</v>
+      </c>
+      <c r="H55">
+        <v>5</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56">
+        <v>2018</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56">
+        <v>10</v>
+      </c>
+      <c r="H56">
+        <v>5</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57">
+        <v>2019</v>
+      </c>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" t="s">
+        <v>59</v>
+      </c>
+      <c r="G57">
+        <v>10</v>
+      </c>
+      <c r="H57">
+        <v>5</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" t="s">
+        <v>60</v>
+      </c>
+      <c r="C58">
+        <v>2021</v>
+      </c>
+      <c r="D58" t="s">
+        <v>61</v>
+      </c>
+      <c r="E58" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58">
+        <v>10</v>
+      </c>
+      <c r="H58">
+        <v>5</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59">
+        <v>2021</v>
+      </c>
+      <c r="D59" t="s">
+        <v>61</v>
+      </c>
+      <c r="E59" t="s">
+        <v>31</v>
+      </c>
+      <c r="G59">
+        <v>10</v>
+      </c>
+      <c r="H59">
+        <v>5</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C60">
+        <v>2021</v>
+      </c>
+      <c r="D60" t="s">
+        <v>61</v>
+      </c>
+      <c r="E60" t="s">
+        <v>54</v>
+      </c>
+      <c r="G60">
+        <v>10</v>
+      </c>
+      <c r="H60">
+        <v>5</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>64</v>
+      </c>
+      <c r="C61">
+        <v>2023</v>
+      </c>
+      <c r="D61" t="s">
+        <v>63</v>
+      </c>
+      <c r="E61" t="s">
+        <v>50</v>
+      </c>
+      <c r="G61">
+        <v>10</v>
+      </c>
+      <c r="H61">
+        <v>5</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J61" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62" t="s">
         <v>65</v>
       </c>
-      <c r="C54">
+      <c r="C62">
         <v>2023</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D62" t="s">
         <v>63</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E62" t="s">
         <v>19</v>
       </c>
-      <c r="G54">
-        <v>10</v>
-      </c>
-      <c r="H54">
-        <v>5</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>70</v>
+      <c r="G62">
+        <v>10</v>
+      </c>
+      <c r="H62">
+        <v>5</v>
+      </c>
+      <c r="I62" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J62" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>2023</v>
+      </c>
+      <c r="D63" t="s">
+        <v>63</v>
+      </c>
+      <c r="E63" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63">
+        <v>10</v>
+      </c>
+      <c r="H63">
+        <v>5</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J63" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J54" xr:uid="{E8C83D10-D6CD-43BE-91E0-25A15ABA6B36}">
-    <filterColumn colId="9">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J63" xr:uid="{E8C83D10-D6CD-43BE-91E0-25A15ABA6B36}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1" xr:uid="{F12C8889-233E-4D88-91CA-82BCF5A31AEA}"/>
-    <hyperlink ref="I3:I11" r:id="rId2" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{4C87EC09-2941-4524-BA3E-34E7D5F375A4}"/>
-    <hyperlink ref="I13:I19" r:id="rId3" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{898171B2-BD9A-4587-AD7F-D353F4E1ECC4}"/>
-    <hyperlink ref="I21:I22" r:id="rId4" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{1B3AFF24-5F39-414B-B0A6-ABF01F35A4C1}"/>
-    <hyperlink ref="I24:I26" r:id="rId5" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{9E46802A-7C66-4114-9F0B-145434CDF86D}"/>
-    <hyperlink ref="I28:I31" r:id="rId6" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{764966E2-E14A-4E57-AF94-FC9C3C3E75EB}"/>
-    <hyperlink ref="I37" r:id="rId7" xr:uid="{1BEAF126-4AAB-4F09-A5D7-9DF756D62051}"/>
-    <hyperlink ref="I39" r:id="rId8" xr:uid="{58C7702E-D0F7-4DA3-93E3-FE80859AC198}"/>
-    <hyperlink ref="I41:I44" r:id="rId9" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{C7A98F58-2C7B-40E0-88A4-8E96B5590279}"/>
-    <hyperlink ref="I46:I54" r:id="rId10" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{265E5F68-79E3-4018-9552-84A370A20CA2}"/>
-    <hyperlink ref="J2" r:id="rId11" xr:uid="{0421CCD1-6112-4B90-B775-FCC691147795}"/>
-    <hyperlink ref="I34" r:id="rId12" xr:uid="{896DD40A-FF0E-49EA-BFF7-67BB43E791D5}"/>
-    <hyperlink ref="I32" r:id="rId13" xr:uid="{E4C0CB5B-012D-4714-9D0B-AD75C1C8570B}"/>
-    <hyperlink ref="J31" r:id="rId14" xr:uid="{644AECA0-A45A-42BE-B259-4D5B68CC57CA}"/>
-    <hyperlink ref="I23" r:id="rId15" xr:uid="{2324BE85-A6C4-4A6B-A8DE-9E4D276406AB}"/>
-    <hyperlink ref="J9" r:id="rId16" xr:uid="{BD8BD086-4106-4457-B4FC-9FB031264A24}"/>
-    <hyperlink ref="I38" r:id="rId17" xr:uid="{83813776-6F4B-464C-B54A-3AC8B8505F93}"/>
-    <hyperlink ref="I40" r:id="rId18" xr:uid="{71D02F04-4915-47BD-A51D-60AA84836D8E}"/>
-    <hyperlink ref="J6" r:id="rId19" xr:uid="{303A4440-5E60-4914-A936-17D2C2165AB4}"/>
-    <hyperlink ref="J35" r:id="rId20" xr:uid="{77DF0A13-DD03-4109-9AEB-AC4A2C7C31CE}"/>
-    <hyperlink ref="J37" r:id="rId21" xr:uid="{6D1DAAF2-6A00-49A9-91A8-0924ADB1785B}"/>
-    <hyperlink ref="I35" r:id="rId22" xr:uid="{37477F18-51BE-4C94-AC4C-C9EADD35F812}"/>
-    <hyperlink ref="I36" r:id="rId23" xr:uid="{F4F1F5F0-1578-4A30-ACE6-2EA9700964F0}"/>
-    <hyperlink ref="J15" r:id="rId24" xr:uid="{A4E2E862-7695-4D30-A310-58165A9BA512}"/>
-    <hyperlink ref="J25" r:id="rId25" xr:uid="{243C2AA1-F6F6-4BDE-92C7-76FAC9FDC489}"/>
-    <hyperlink ref="J41" r:id="rId26" xr:uid="{8113FD18-FFDA-4C84-B4C7-2E9488300A46}"/>
-    <hyperlink ref="J47" r:id="rId27" xr:uid="{E85DD121-2527-4027-B243-BC55C0622959}"/>
-    <hyperlink ref="I12" r:id="rId28" xr:uid="{83F45C64-E30E-440B-9947-687857F6FF6A}"/>
-    <hyperlink ref="J8" r:id="rId29" xr:uid="{D7C9493B-D00C-4E90-8D04-7CF17A6D8A52}"/>
-    <hyperlink ref="J13" r:id="rId30" xr:uid="{FEBA08E4-8E03-456E-918A-C58214BFDC6A}"/>
-    <hyperlink ref="J29" r:id="rId31" xr:uid="{653F89C2-252F-4AC8-9A56-B19C62575535}"/>
-    <hyperlink ref="J44" r:id="rId32" xr:uid="{A4F7AD98-5E16-47DC-9935-3A51361A6286}"/>
-    <hyperlink ref="J48" r:id="rId33" xr:uid="{C8270984-A5B6-424B-AFE6-A1620FD61B26}"/>
-    <hyperlink ref="I27" r:id="rId34" xr:uid="{FB5C7A0A-C319-4C33-82E9-F73E9BF4C3EA}"/>
-    <hyperlink ref="I45" r:id="rId35" xr:uid="{FD6511FA-45E1-44A0-8BFE-925EA5DA45DB}"/>
-    <hyperlink ref="J26" r:id="rId36" xr:uid="{1587D7F5-2F89-4911-A322-94401912B480}"/>
-    <hyperlink ref="I33" r:id="rId37" xr:uid="{47D58433-DD09-40A9-833F-2A6807061734}"/>
-    <hyperlink ref="J32" r:id="rId38" xr:uid="{730E8753-7938-46CD-80C6-9FC4C62C05E6}"/>
-    <hyperlink ref="I20" r:id="rId39" xr:uid="{65FF6849-86C2-4EE7-B047-C3FC0C3A9C1E}"/>
-    <hyperlink ref="J3" r:id="rId40" xr:uid="{78EA83B8-A90E-4C38-ADF5-A381AE6620EC}"/>
-    <hyperlink ref="J5" r:id="rId41" xr:uid="{8AFDEA20-0725-4C32-9267-8826CD8AFA38}"/>
+    <hyperlink ref="I3:I12" r:id="rId2" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{4C87EC09-2941-4524-BA3E-34E7D5F375A4}"/>
+    <hyperlink ref="I14:I24" r:id="rId3" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{898171B2-BD9A-4587-AD7F-D353F4E1ECC4}"/>
+    <hyperlink ref="I26:I27" r:id="rId4" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{1B3AFF24-5F39-414B-B0A6-ABF01F35A4C1}"/>
+    <hyperlink ref="I29:I31" r:id="rId5" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{9E46802A-7C66-4114-9F0B-145434CDF86D}"/>
+    <hyperlink ref="I33:I36" r:id="rId6" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{764966E2-E14A-4E57-AF94-FC9C3C3E75EB}"/>
+    <hyperlink ref="I44" r:id="rId7" xr:uid="{1BEAF126-4AAB-4F09-A5D7-9DF756D62051}"/>
+    <hyperlink ref="I46" r:id="rId8" xr:uid="{58C7702E-D0F7-4DA3-93E3-FE80859AC198}"/>
+    <hyperlink ref="I48:I51" r:id="rId9" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{C7A98F58-2C7B-40E0-88A4-8E96B5590279}"/>
+    <hyperlink ref="I53:I62" r:id="rId10" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{265E5F68-79E3-4018-9552-84A370A20CA2}"/>
+    <hyperlink ref="I39" r:id="rId11" xr:uid="{896DD40A-FF0E-49EA-BFF7-67BB43E791D5}"/>
+    <hyperlink ref="J36" r:id="rId12" xr:uid="{644AECA0-A45A-42BE-B259-4D5B68CC57CA}"/>
+    <hyperlink ref="I45" r:id="rId13" xr:uid="{83813776-6F4B-464C-B54A-3AC8B8505F93}"/>
+    <hyperlink ref="J6" r:id="rId14" xr:uid="{303A4440-5E60-4914-A936-17D2C2165AB4}"/>
+    <hyperlink ref="I25" r:id="rId15" xr:uid="{65FF6849-86C2-4EE7-B047-C3FC0C3A9C1E}"/>
+    <hyperlink ref="J3" r:id="rId16" xr:uid="{78EA83B8-A90E-4C38-ADF5-A381AE6620EC}"/>
+    <hyperlink ref="J2" r:id="rId17" xr:uid="{5748E202-0610-4429-B59C-C85B45D21A38}"/>
+    <hyperlink ref="J4" r:id="rId18" xr:uid="{B9C5815E-C91F-4822-A60B-26ABC9D18B7A}"/>
+    <hyperlink ref="J7" r:id="rId19" xr:uid="{585A9E42-6570-4436-82E7-0D9BEA208035}"/>
+    <hyperlink ref="J13" r:id="rId20" xr:uid="{EE4CEE3B-33D1-4373-A76F-F593B224A1B3}"/>
+    <hyperlink ref="I63" r:id="rId21" xr:uid="{8BFFACAD-FAD6-405E-B992-C4A0051C18EE}"/>
+    <hyperlink ref="J63" r:id="rId22" xr:uid="{9998AC0F-FA20-4EFC-B740-6510A5F88C01}"/>
+    <hyperlink ref="I32" r:id="rId23" xr:uid="{62EC85A5-87F0-4348-AE5C-CE2ECAC5B4FE}"/>
+    <hyperlink ref="I52" r:id="rId24" xr:uid="{4720AF8A-287A-4FDC-8E47-A448C3AC3E82}"/>
+    <hyperlink ref="J31" r:id="rId25" xr:uid="{9DE2DCDC-76C5-4F67-842D-6BDECB77345A}"/>
+    <hyperlink ref="I37" r:id="rId26" xr:uid="{2080A826-3145-4186-8445-97B7EEB1AB71}"/>
+    <hyperlink ref="I42" r:id="rId27" xr:uid="{60D8C41E-67B5-47E4-8046-A73519D62041}"/>
+    <hyperlink ref="I43" r:id="rId28" xr:uid="{417A47FF-B3E4-4A6C-B84E-7CFDD9D6229E}"/>
+    <hyperlink ref="J16" r:id="rId29" xr:uid="{DD176412-7E49-4295-96A3-1D25E4F64725}"/>
+    <hyperlink ref="J30" r:id="rId30" xr:uid="{A2D82066-C73E-4108-A5D5-27FB4BD16F6C}"/>
+    <hyperlink ref="J48" r:id="rId31" xr:uid="{7A91FC10-44E5-4A1A-8DEC-CAEC33929B0F}"/>
+    <hyperlink ref="J55" r:id="rId32" xr:uid="{6335DA8F-CF08-4974-A527-F506BDE8D0F5}"/>
+    <hyperlink ref="I13" r:id="rId33" xr:uid="{748ADAD2-77C0-4CC4-9EDC-90D46D705749}"/>
+    <hyperlink ref="J8" r:id="rId34" xr:uid="{CC624DA3-8194-4F8E-A622-C4A7BBF91D03}"/>
+    <hyperlink ref="J14" r:id="rId35" xr:uid="{FC541377-2AEA-4DA6-8E18-F7E360E14921}"/>
+    <hyperlink ref="J34" r:id="rId36" xr:uid="{7B42B139-A34D-4BC3-8267-12D19B9DA4F5}"/>
+    <hyperlink ref="J51" r:id="rId37" xr:uid="{0F2FBBA9-5A51-4F69-9755-F3438AAE10D6}"/>
+    <hyperlink ref="J56" r:id="rId38" xr:uid="{711667BA-3C30-4FE7-9826-94C9A946E1E3}"/>
+    <hyperlink ref="I47" r:id="rId39" xr:uid="{01F6FC46-9E85-462A-84A3-19ECCABC0426}"/>
+    <hyperlink ref="J42" r:id="rId40" xr:uid="{7721FC71-0048-4CE0-997A-67BD6004E684}"/>
+    <hyperlink ref="J44" r:id="rId41" xr:uid="{EB742833-2097-44BE-9C21-2DC83CF7859D}"/>
+    <hyperlink ref="I38" r:id="rId42" xr:uid="{979313BD-650F-49B8-91A4-3A95F6B0DB6C}"/>
+    <hyperlink ref="J37" r:id="rId43" xr:uid="{3BB36A31-71A0-4E57-938A-4F4BA60DB93A}"/>
+    <hyperlink ref="J5" r:id="rId44" xr:uid="{39BF4239-7AA4-42ED-B651-C0A9ABC85D36}"/>
+    <hyperlink ref="I28" r:id="rId45" xr:uid="{0046B2D3-E3BE-421B-96C2-712DFC40A195}"/>
+    <hyperlink ref="J9" r:id="rId46" xr:uid="{7A007FA7-06FA-4572-8A33-6A9EC04169B6}"/>
+    <hyperlink ref="J24" r:id="rId47" xr:uid="{A716DA10-3F64-4353-832D-5D65973EA357}"/>
+    <hyperlink ref="J25" r:id="rId48" xr:uid="{DE03A91C-86C3-46D7-A3F9-8B0F6D1C48BB}"/>
+    <hyperlink ref="J27" r:id="rId49" xr:uid="{7737FA32-A017-494D-9612-4B930F7FF9B4}"/>
+    <hyperlink ref="J28" r:id="rId50" xr:uid="{284CBC0D-E0B1-456B-B49D-3AEB25A0AC04}"/>
+    <hyperlink ref="J17" r:id="rId51" xr:uid="{E7BF36E1-0B4C-4204-AA0C-016C1194BF53}"/>
+    <hyperlink ref="J29" r:id="rId52" xr:uid="{60E6BF30-948D-4862-B9CA-C0738F854E13}"/>
+    <hyperlink ref="J39" r:id="rId53" xr:uid="{0445726A-BEF0-4202-A562-F62388E532CF}"/>
+    <hyperlink ref="J26" r:id="rId54" xr:uid="{164C9F20-1327-4609-8306-753F2FBC4930}"/>
+    <hyperlink ref="J18" r:id="rId55" xr:uid="{ECEC2631-F779-4C3E-8023-F797689B1BA7}"/>
+    <hyperlink ref="J23" r:id="rId56" xr:uid="{C2763E50-45C0-4F49-8C71-948FEFE4A5BA}"/>
+    <hyperlink ref="J32" r:id="rId57" xr:uid="{F3C17C06-C75D-4B30-9184-4C7F2AB3A3EB}"/>
+    <hyperlink ref="J33" r:id="rId58" xr:uid="{1F13BDD3-773C-4D6F-A9FF-D7368D22E426}"/>
+    <hyperlink ref="J52" r:id="rId59" xr:uid="{D0649255-1AF8-4852-8F0A-71747BBD0561}"/>
+    <hyperlink ref="J12" r:id="rId60" xr:uid="{0EB448E5-33A1-4F8A-AEA1-96FA4D894100}"/>
+    <hyperlink ref="J15" r:id="rId61" xr:uid="{6C681A6F-5BC3-4A2E-8803-B47814E3E649}"/>
+    <hyperlink ref="J10" r:id="rId62" xr:uid="{4D1F60AD-0F12-4248-9EDC-0342FA3A9E16}"/>
+    <hyperlink ref="J38" r:id="rId63" xr:uid="{BC8AF356-2712-4561-8768-7BDA19739073}"/>
+    <hyperlink ref="J35" r:id="rId64" xr:uid="{C17B5985-7F10-490B-89A4-E439DF52E2D3}"/>
+    <hyperlink ref="J50" r:id="rId65" xr:uid="{D600D3FF-C4CA-4323-A73D-DC6D1B8D3263}"/>
+    <hyperlink ref="J53" r:id="rId66" xr:uid="{30B3E14A-A8B0-4A72-9691-52AEC023D3AE}"/>
+    <hyperlink ref="J60" r:id="rId67" xr:uid="{DD47E6AB-3F10-4CC4-9665-5B9F4CAA251D}"/>
+    <hyperlink ref="J45" r:id="rId68" xr:uid="{F4A211EA-3FF2-4EB9-A49B-69416581C321}"/>
+    <hyperlink ref="J46" r:id="rId69" xr:uid="{986F8FEB-9DE0-4C83-9556-D21C1798D8A6}"/>
+    <hyperlink ref="J58" r:id="rId70" xr:uid="{022F3606-06A3-4750-BD88-1AC2F0D1DE52}"/>
+    <hyperlink ref="J43" r:id="rId71" xr:uid="{F980623A-7913-43A5-9A5C-0D3022386A08}"/>
+    <hyperlink ref="J47" r:id="rId72" xr:uid="{68D9F805-EC8D-4A66-A0A7-61A3F69F46AB}"/>
+    <hyperlink ref="J57" r:id="rId73" xr:uid="{4EA12311-DDCC-48D4-A6BA-4D99903BD541}"/>
+    <hyperlink ref="J49" r:id="rId74" xr:uid="{C47A4DFD-8B04-4A3A-A436-BB9C62EE48C5}"/>
+    <hyperlink ref="J59" r:id="rId75" xr:uid="{D6F34887-786B-4CDA-8BFA-F4870D073135}"/>
+    <hyperlink ref="J62" r:id="rId76" xr:uid="{2E4ED292-FC0F-41AD-A5B9-BC08DA52292D}"/>
+    <hyperlink ref="J61" r:id="rId77" xr:uid="{821D41D1-C558-4CA8-BC7B-16B6D0659D57}"/>
+    <hyperlink ref="I11" r:id="rId78" xr:uid="{9A2AC793-323E-49DC-AADB-A40B62E24402}"/>
+    <hyperlink ref="J11" r:id="rId79" xr:uid="{F7E882AD-67A4-4270-896B-E583B45947B6}"/>
+    <hyperlink ref="I19" r:id="rId80" xr:uid="{D18B1282-5727-4E67-AA19-8989266BAB08}"/>
+    <hyperlink ref="J19" r:id="rId81" xr:uid="{D5F976F5-D97D-463A-BB78-8D5E4FED278A}"/>
+    <hyperlink ref="I20" r:id="rId82" xr:uid="{5C3C1709-91B8-4BAC-AB28-C8DD467CCC4F}"/>
+    <hyperlink ref="J20" r:id="rId83" xr:uid="{6EAEAC19-9EDA-4892-951C-44E664980DCB}"/>
+    <hyperlink ref="I21" r:id="rId84" xr:uid="{0E186AEA-136D-410F-921B-761211D73F45}"/>
+    <hyperlink ref="J21" r:id="rId85" xr:uid="{474962BC-622D-4BAA-9CA6-C7456D566E8E}"/>
+    <hyperlink ref="I22" r:id="rId86" xr:uid="{109F245F-78CD-48BD-A5D6-AC7D52C505E7}"/>
+    <hyperlink ref="J22" r:id="rId87" xr:uid="{A1138993-1484-441C-B80E-4E404A8EC04D}"/>
+    <hyperlink ref="I40" r:id="rId88" xr:uid="{87F589F1-50D5-4079-A71A-6CC9D6BA86E2}"/>
+    <hyperlink ref="J40" r:id="rId89" xr:uid="{491FE978-A405-4646-8B13-99EF19506C42}"/>
+    <hyperlink ref="I41" r:id="rId90" xr:uid="{8B6679C5-F52C-4450-83EF-5B1DA246AD68}"/>
+    <hyperlink ref="J41" r:id="rId91" xr:uid="{E262CD59-EDED-4B97-99FB-AEAAB34F008F}"/>
+    <hyperlink ref="I54" r:id="rId92" xr:uid="{9E106DDF-E9B7-48B3-9F2C-A634E58FD444}"/>
+    <hyperlink ref="J54" r:id="rId93" xr:uid="{F047EC1B-3060-4740-B4A2-1E512C1A0D7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId94"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add final changes to social dashboard
</commit_message>
<xml_diff>
--- a/files/beef.xlsx
+++ b/files/beef.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marin\Desktop\Adalab\Pair-Programming\Modulo-4\promog-modulo4-sprint2-pairprogramming-marina_escobar-isabel_correal\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7513730-F8DA-4001-802C-399116651ECD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C87ACE-8B74-4D8D-A324-E2DFB2D76719}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{BE06563D-F197-4548-8C70-5C4CDDF48CD1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$70</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="132">
   <si>
     <t>Source</t>
   </si>
@@ -397,6 +397,42 @@
   </si>
   <si>
     <t>Amigo (Taylor)</t>
+  </si>
+  <si>
+    <t>Folklore</t>
+  </si>
+  <si>
+    <t>Evermore</t>
+  </si>
+  <si>
+    <t>Sophie Turner</t>
+  </si>
+  <si>
+    <t>Expareja (Taylor) / Expareja (Gigi)</t>
+  </si>
+  <si>
+    <t>Amiga (Taylor) / Expareja (Joe)</t>
+  </si>
+  <si>
+    <t>Expareja (Taylor) / Expareja (Gigi) / Marido (Sophie)</t>
+  </si>
+  <si>
+    <t>Amiga (Taylor) / Mujer (Joe)</t>
+  </si>
+  <si>
+    <t>Amiga (Taylor) / Exmarido (Joe)</t>
+  </si>
+  <si>
+    <t>Amiga (Taylor) / Exmujer (Joe)</t>
+  </si>
+  <si>
+    <t>Expareja (Taylor) / Expareja (Gigi) / Exmarido (Sophie)</t>
+  </si>
+  <si>
+    <t>https://i.imgur.com/IUuJEy2.jpeg</t>
+  </si>
+  <si>
+    <t>Examiga (Taylor)</t>
   </si>
 </sst>
 </file>
@@ -765,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C83D10-D6CD-43BE-91E0-25A15ABA6B36}">
-  <dimension ref="A1:K64"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1169,7 @@
         <v>2010</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F12" t="s">
         <v>95</v>
@@ -1661,16 +1697,16 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="C30">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="D30">
         <v>1989</v>
       </c>
       <c r="F30" t="s">
-        <v>100</v>
+        <v>131</v>
       </c>
       <c r="H30">
         <v>10</v>
@@ -1682,7 +1718,7 @@
         <v>53</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -1690,7 +1726,7 @@
         <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>2014</v>
@@ -1699,10 +1735,7 @@
         <v>1989</v>
       </c>
       <c r="F31" t="s">
-        <v>90</v>
-      </c>
-      <c r="G31" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="H31">
         <v>10</v>
@@ -1714,7 +1747,7 @@
         <v>53</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -1722,7 +1755,7 @@
         <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="C32">
         <v>2014</v>
@@ -1731,7 +1764,10 @@
         <v>1989</v>
       </c>
       <c r="F32" t="s">
-        <v>104</v>
+        <v>90</v>
+      </c>
+      <c r="G32" t="s">
+        <v>29</v>
       </c>
       <c r="H32">
         <v>10</v>
@@ -1743,15 +1779,15 @@
         <v>53</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
         <v>27</v>
-      </c>
-      <c r="B33" t="s">
-        <v>28</v>
       </c>
       <c r="C33">
         <v>2014</v>
@@ -1759,12 +1795,9 @@
       <c r="D33">
         <v>1989</v>
       </c>
-      <c r="E33" t="s">
+      <c r="F33" t="s">
         <v>104</v>
       </c>
-      <c r="F33" t="s">
-        <v>105</v>
-      </c>
       <c r="H33">
         <v>10</v>
       </c>
@@ -1772,15 +1805,15 @@
         <v>5</v>
       </c>
       <c r="J33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
         <v>28</v>
@@ -1791,6 +1824,9 @@
       <c r="D34">
         <v>1989</v>
       </c>
+      <c r="E34" t="s">
+        <v>104</v>
+      </c>
       <c r="F34" t="s">
         <v>105</v>
       </c>
@@ -1801,7 +1837,7 @@
         <v>5</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>71</v>
@@ -1812,7 +1848,7 @@
         <v>3</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="C35">
         <v>2014</v>
@@ -1821,7 +1857,7 @@
         <v>1989</v>
       </c>
       <c r="F35" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H35">
         <v>10</v>
@@ -1833,7 +1869,7 @@
         <v>53</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1841,19 +1877,16 @@
         <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C36">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D36">
         <v>1989</v>
       </c>
       <c r="F36" t="s">
-        <v>92</v>
-      </c>
-      <c r="G36" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="H36">
         <v>10</v>
@@ -1865,7 +1898,7 @@
         <v>53</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -1873,7 +1906,7 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C37">
         <v>2015</v>
@@ -1882,7 +1915,7 @@
         <v>1989</v>
       </c>
       <c r="F37" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
         <v>30</v>
@@ -1897,15 +1930,15 @@
         <v>53</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
         <v>32</v>
-      </c>
-      <c r="B38" t="s">
-        <v>33</v>
       </c>
       <c r="C38">
         <v>2015</v>
@@ -1913,11 +1946,8 @@
       <c r="D38">
         <v>1989</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>106</v>
-      </c>
-      <c r="F38" t="s">
-        <v>107</v>
       </c>
       <c r="G38" t="s">
         <v>30</v>
@@ -1929,18 +1959,18 @@
         <v>5</v>
       </c>
       <c r="J38" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K38" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" t="s">
         <v>33</v>
-      </c>
-      <c r="B39" t="s">
-        <v>14</v>
       </c>
       <c r="C39">
         <v>2015</v>
@@ -1949,10 +1979,10 @@
         <v>1989</v>
       </c>
       <c r="E39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" t="s">
         <v>107</v>
-      </c>
-      <c r="F39" t="s">
-        <v>108</v>
       </c>
       <c r="G39" t="s">
         <v>30</v>
@@ -1964,18 +1994,18 @@
         <v>5</v>
       </c>
       <c r="J39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C40">
         <v>2015</v>
@@ -1984,10 +2014,10 @@
         <v>1989</v>
       </c>
       <c r="E40" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="F40" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G40" t="s">
         <v>30</v>
@@ -1999,27 +2029,33 @@
         <v>5</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41">
-        <v>2016</v>
-      </c>
-      <c r="D41" t="s">
-        <v>34</v>
+        <v>2015</v>
+      </c>
+      <c r="D41">
+        <v>1989</v>
+      </c>
+      <c r="E41" t="s">
+        <v>123</v>
       </c>
       <c r="F41" t="s">
-        <v>111</v>
+        <v>124</v>
+      </c>
+      <c r="G41" t="s">
+        <v>30</v>
       </c>
       <c r="H41">
         <v>10</v>
@@ -2028,10 +2064,10 @@
         <v>5</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -2039,7 +2075,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C42">
         <v>2016</v>
@@ -2048,7 +2084,7 @@
         <v>34</v>
       </c>
       <c r="F42" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H42">
         <v>10</v>
@@ -2060,15 +2096,15 @@
         <v>53</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C43">
         <v>2016</v>
@@ -2076,14 +2112,8 @@
       <c r="D43" t="s">
         <v>34</v>
       </c>
-      <c r="E43" t="s">
-        <v>115</v>
-      </c>
       <c r="F43" t="s">
-        <v>113</v>
-      </c>
-      <c r="G43" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="H43">
         <v>10</v>
@@ -2092,10 +2122,10 @@
         <v>5</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2103,7 +2133,7 @@
         <v>16</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <v>2016</v>
@@ -2115,7 +2145,10 @@
         <v>115</v>
       </c>
       <c r="F44" t="s">
-        <v>116</v>
+        <v>113</v>
+      </c>
+      <c r="G44" t="s">
+        <v>35</v>
       </c>
       <c r="H44">
         <v>10</v>
@@ -2127,15 +2160,15 @@
         <v>58</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C45">
         <v>2016</v>
@@ -2143,8 +2176,11 @@
       <c r="D45" t="s">
         <v>34</v>
       </c>
+      <c r="E45" t="s">
+        <v>115</v>
+      </c>
       <c r="F45" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H45">
         <v>10</v>
@@ -2153,18 +2189,18 @@
         <v>5</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>3</v>
+      </c>
+      <c r="B46" t="s">
         <v>7</v>
-      </c>
-      <c r="B46" t="s">
-        <v>37</v>
       </c>
       <c r="C46">
         <v>2016</v>
@@ -2172,11 +2208,8 @@
       <c r="D46" t="s">
         <v>34</v>
       </c>
-      <c r="E46" t="s">
-        <v>117</v>
-      </c>
       <c r="F46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H46">
         <v>10</v>
@@ -2185,15 +2218,15 @@
         <v>5</v>
       </c>
       <c r="J46" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B47" t="s">
         <v>37</v>
@@ -2204,6 +2237,9 @@
       <c r="D47" t="s">
         <v>34</v>
       </c>
+      <c r="E47" t="s">
+        <v>117</v>
+      </c>
       <c r="F47" t="s">
         <v>114</v>
       </c>
@@ -2214,7 +2250,7 @@
         <v>5</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>76</v>
@@ -2222,10 +2258,10 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C48">
         <v>2016</v>
@@ -2233,11 +2269,8 @@
       <c r="D48" t="s">
         <v>34</v>
       </c>
-      <c r="E48" t="s">
-        <v>117</v>
-      </c>
       <c r="F48" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H48">
         <v>10</v>
@@ -2246,18 +2279,18 @@
         <v>5</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C49">
         <v>2016</v>
@@ -2265,8 +2298,11 @@
       <c r="D49" t="s">
         <v>34</v>
       </c>
+      <c r="E49" t="s">
+        <v>117</v>
+      </c>
       <c r="F49" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H49">
         <v>10</v>
@@ -2275,10 +2311,10 @@
         <v>5</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -2286,7 +2322,7 @@
         <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="C50">
         <v>2016</v>
@@ -2295,7 +2331,7 @@
         <v>34</v>
       </c>
       <c r="F50" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="H50">
         <v>10</v>
@@ -2307,7 +2343,7 @@
         <v>53</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -2315,7 +2351,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C51">
         <v>2016</v>
@@ -2336,7 +2372,7 @@
         <v>53</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -2344,7 +2380,7 @@
         <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="C52">
         <v>2016</v>
@@ -2353,10 +2389,7 @@
         <v>34</v>
       </c>
       <c r="F52" t="s">
-        <v>118</v>
-      </c>
-      <c r="G52" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="H52">
         <v>10</v>
@@ -2368,27 +2401,27 @@
         <v>53</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C53">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="D53" t="s">
         <v>34</v>
       </c>
-      <c r="E53" t="s">
-        <v>111</v>
-      </c>
       <c r="F53" t="s">
-        <v>112</v>
+        <v>118</v>
+      </c>
+      <c r="G53" t="s">
+        <v>39</v>
       </c>
       <c r="H53">
         <v>10</v>
@@ -2397,18 +2430,18 @@
         <v>5</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>3</v>
+        <v>27</v>
       </c>
       <c r="B54" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C54">
         <v>2017</v>
@@ -2416,8 +2449,11 @@
       <c r="D54" t="s">
         <v>34</v>
       </c>
+      <c r="E54" t="s">
+        <v>111</v>
+      </c>
       <c r="F54" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="H54">
         <v>10</v>
@@ -2426,30 +2462,27 @@
         <v>5</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C55">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
-      </c>
-      <c r="E55" t="s">
-        <v>110</v>
+        <v>34</v>
       </c>
       <c r="F55" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="H55">
         <v>10</v>
@@ -2458,18 +2491,18 @@
         <v>5</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B56" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C56">
         <v>2018</v>
@@ -2477,8 +2510,11 @@
       <c r="D56" t="s">
         <v>41</v>
       </c>
+      <c r="E56" t="s">
+        <v>110</v>
+      </c>
       <c r="F56" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H56">
         <v>10</v>
@@ -2487,10 +2523,10 @@
         <v>5</v>
       </c>
       <c r="J56" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="K56" s="1" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -2498,7 +2534,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C57">
         <v>2018</v>
@@ -2507,7 +2543,7 @@
         <v>41</v>
       </c>
       <c r="F57" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="H57">
         <v>10</v>
@@ -2519,7 +2555,7 @@
         <v>53</v>
       </c>
       <c r="K57" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -2527,19 +2563,16 @@
         <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C58">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D58" t="s">
         <v>41</v>
       </c>
       <c r="F58" t="s">
-        <v>109</v>
-      </c>
-      <c r="G58" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="H58">
         <v>10</v>
@@ -2551,7 +2584,7 @@
         <v>53</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -2559,16 +2592,19 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C59">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="D59" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F59" t="s">
-        <v>86</v>
+        <v>109</v>
+      </c>
+      <c r="G59" t="s">
+        <v>42</v>
       </c>
       <c r="H59">
         <v>10</v>
@@ -2580,7 +2616,7 @@
         <v>53</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -2588,16 +2624,16 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C60">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D60" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="F60" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="H60">
         <v>10</v>
@@ -2609,7 +2645,7 @@
         <v>53</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -2620,13 +2656,13 @@
         <v>40</v>
       </c>
       <c r="C61">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="D61" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="F61" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="H61">
         <v>10</v>
@@ -2646,16 +2682,16 @@
         <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>47</v>
+        <v>122</v>
       </c>
       <c r="C62">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="D62" t="s">
-        <v>46</v>
+        <v>120</v>
       </c>
       <c r="F62" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="H62">
         <v>10</v>
@@ -2667,24 +2703,27 @@
         <v>53</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="C63">
-        <v>2023</v>
+        <v>2020</v>
       </c>
       <c r="D63" t="s">
-        <v>46</v>
+        <v>120</v>
+      </c>
+      <c r="E63" t="s">
+        <v>125</v>
       </c>
       <c r="F63" t="s">
-        <v>86</v>
+        <v>126</v>
       </c>
       <c r="H63">
         <v>10</v>
@@ -2693,10 +2732,10 @@
         <v>5</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -2704,132 +2743,413 @@
         <v>3</v>
       </c>
       <c r="B64" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64">
+        <v>2020</v>
+      </c>
+      <c r="D64" t="s">
+        <v>120</v>
+      </c>
+      <c r="F64" t="s">
+        <v>129</v>
+      </c>
+      <c r="H64">
+        <v>10</v>
+      </c>
+      <c r="I64">
+        <v>5</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65">
+        <v>2021</v>
+      </c>
+      <c r="D65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>86</v>
+      </c>
+      <c r="H65">
+        <v>10</v>
+      </c>
+      <c r="I65">
+        <v>5</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66">
+        <v>2021</v>
+      </c>
+      <c r="D66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" t="s">
+        <v>103</v>
+      </c>
+      <c r="H66">
+        <v>10</v>
+      </c>
+      <c r="I66">
+        <v>5</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67">
+        <v>2021</v>
+      </c>
+      <c r="D67" t="s">
+        <v>44</v>
+      </c>
+      <c r="F67" t="s">
+        <v>95</v>
+      </c>
+      <c r="H67">
+        <v>10</v>
+      </c>
+      <c r="I67">
+        <v>5</v>
+      </c>
+      <c r="J67" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68">
+        <v>2023</v>
+      </c>
+      <c r="D68" t="s">
+        <v>46</v>
+      </c>
+      <c r="F68" t="s">
+        <v>92</v>
+      </c>
+      <c r="H68">
+        <v>10</v>
+      </c>
+      <c r="I68">
+        <v>5</v>
+      </c>
+      <c r="J68" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K68" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" t="s">
+        <v>48</v>
+      </c>
+      <c r="C69">
+        <v>2023</v>
+      </c>
+      <c r="D69" t="s">
+        <v>46</v>
+      </c>
+      <c r="F69" t="s">
+        <v>86</v>
+      </c>
+      <c r="H69">
+        <v>10</v>
+      </c>
+      <c r="I69">
+        <v>5</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70" t="s">
         <v>6</v>
       </c>
-      <c r="C64">
+      <c r="C70">
         <v>2023</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D70" t="s">
         <v>46</v>
       </c>
-      <c r="F64" t="s">
+      <c r="F70" t="s">
         <v>119</v>
       </c>
-      <c r="H64">
-        <v>10</v>
-      </c>
-      <c r="I64">
-        <v>5</v>
-      </c>
-      <c r="J64" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K64" s="1" t="s">
+      <c r="H70">
+        <v>10</v>
+      </c>
+      <c r="I70">
+        <v>5</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K70" s="1" t="s">
         <v>61</v>
       </c>
     </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71">
+        <v>2023</v>
+      </c>
+      <c r="D71" t="s">
+        <v>46</v>
+      </c>
+      <c r="F71" t="s">
+        <v>127</v>
+      </c>
+      <c r="H71">
+        <v>10</v>
+      </c>
+      <c r="I71">
+        <v>5</v>
+      </c>
+      <c r="J71" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72" t="s">
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <v>2023</v>
+      </c>
+      <c r="D72" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" t="s">
+        <v>129</v>
+      </c>
+      <c r="H72">
+        <v>10</v>
+      </c>
+      <c r="I72">
+        <v>5</v>
+      </c>
+      <c r="J72" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K72" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73">
+        <v>2023</v>
+      </c>
+      <c r="D73" t="s">
+        <v>46</v>
+      </c>
+      <c r="E73" t="s">
+        <v>129</v>
+      </c>
+      <c r="F73" t="s">
+        <v>128</v>
+      </c>
+      <c r="H73">
+        <v>10</v>
+      </c>
+      <c r="I73">
+        <v>5</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K64" xr:uid="{E8C83D10-D6CD-43BE-91E0-25A15ABA6B36}"/>
+  <autoFilter ref="A1:K70" xr:uid="{E8C83D10-D6CD-43BE-91E0-25A15ABA6B36}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="J4" r:id="rId1" xr:uid="{F12C8889-233E-4D88-91CA-82BCF5A31AEA}"/>
     <hyperlink ref="J5:J13" r:id="rId2" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{4C87EC09-2941-4524-BA3E-34E7D5F375A4}"/>
     <hyperlink ref="J15:J25" r:id="rId3" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{898171B2-BD9A-4587-AD7F-D353F4E1ECC4}"/>
     <hyperlink ref="J27:J28" r:id="rId4" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{1B3AFF24-5F39-414B-B0A6-ABF01F35A4C1}"/>
-    <hyperlink ref="J30:J32" r:id="rId5" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{9E46802A-7C66-4114-9F0B-145434CDF86D}"/>
-    <hyperlink ref="J34:J37" r:id="rId6" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{764966E2-E14A-4E57-AF94-FC9C3C3E75EB}"/>
-    <hyperlink ref="J45" r:id="rId7" xr:uid="{1BEAF126-4AAB-4F09-A5D7-9DF756D62051}"/>
-    <hyperlink ref="J47" r:id="rId8" xr:uid="{58C7702E-D0F7-4DA3-93E3-FE80859AC198}"/>
-    <hyperlink ref="J49:J52" r:id="rId9" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{C7A98F58-2C7B-40E0-88A4-8E96B5590279}"/>
-    <hyperlink ref="J54:J63" r:id="rId10" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{265E5F68-79E3-4018-9552-84A370A20CA2}"/>
-    <hyperlink ref="J40" r:id="rId11" xr:uid="{896DD40A-FF0E-49EA-BFF7-67BB43E791D5}"/>
-    <hyperlink ref="K37" r:id="rId12" xr:uid="{644AECA0-A45A-42BE-B259-4D5B68CC57CA}"/>
-    <hyperlink ref="J46" r:id="rId13" xr:uid="{83813776-6F4B-464C-B54A-3AC8B8505F93}"/>
-    <hyperlink ref="K8" r:id="rId14" xr:uid="{303A4440-5E60-4914-A936-17D2C2165AB4}"/>
-    <hyperlink ref="J26" r:id="rId15" xr:uid="{65FF6849-86C2-4EE7-B047-C3FC0C3A9C1E}"/>
-    <hyperlink ref="K5" r:id="rId16" xr:uid="{78EA83B8-A90E-4C38-ADF5-A381AE6620EC}"/>
-    <hyperlink ref="K4" r:id="rId17" xr:uid="{5748E202-0610-4429-B59C-C85B45D21A38}"/>
-    <hyperlink ref="K6" r:id="rId18" xr:uid="{B9C5815E-C91F-4822-A60B-26ABC9D18B7A}"/>
-    <hyperlink ref="K9" r:id="rId19" xr:uid="{585A9E42-6570-4436-82E7-0D9BEA208035}"/>
-    <hyperlink ref="K14" r:id="rId20" xr:uid="{EE4CEE3B-33D1-4373-A76F-F593B224A1B3}"/>
-    <hyperlink ref="J64" r:id="rId21" xr:uid="{8BFFACAD-FAD6-405E-B992-C4A0051C18EE}"/>
-    <hyperlink ref="K64" r:id="rId22" xr:uid="{9998AC0F-FA20-4EFC-B740-6510A5F88C01}"/>
-    <hyperlink ref="J33" r:id="rId23" xr:uid="{62EC85A5-87F0-4348-AE5C-CE2ECAC5B4FE}"/>
-    <hyperlink ref="J53" r:id="rId24" xr:uid="{4720AF8A-287A-4FDC-8E47-A448C3AC3E82}"/>
-    <hyperlink ref="K32" r:id="rId25" xr:uid="{9DE2DCDC-76C5-4F67-842D-6BDECB77345A}"/>
-    <hyperlink ref="J38" r:id="rId26" xr:uid="{2080A826-3145-4186-8445-97B7EEB1AB71}"/>
-    <hyperlink ref="J43" r:id="rId27" xr:uid="{60D8C41E-67B5-47E4-8046-A73519D62041}"/>
-    <hyperlink ref="J44" r:id="rId28" xr:uid="{417A47FF-B3E4-4A6C-B84E-7CFDD9D6229E}"/>
-    <hyperlink ref="K17" r:id="rId29" xr:uid="{DD176412-7E49-4295-96A3-1D25E4F64725}"/>
-    <hyperlink ref="K31" r:id="rId30" xr:uid="{A2D82066-C73E-4108-A5D5-27FB4BD16F6C}"/>
-    <hyperlink ref="K49" r:id="rId31" xr:uid="{7A91FC10-44E5-4A1A-8DEC-CAEC33929B0F}"/>
-    <hyperlink ref="K56" r:id="rId32" xr:uid="{6335DA8F-CF08-4974-A527-F506BDE8D0F5}"/>
-    <hyperlink ref="J14" r:id="rId33" xr:uid="{748ADAD2-77C0-4CC4-9EDC-90D46D705749}"/>
-    <hyperlink ref="K10" r:id="rId34" xr:uid="{CC624DA3-8194-4F8E-A622-C4A7BBF91D03}"/>
-    <hyperlink ref="K15" r:id="rId35" xr:uid="{FC541377-2AEA-4DA6-8E18-F7E360E14921}"/>
-    <hyperlink ref="K35" r:id="rId36" xr:uid="{7B42B139-A34D-4BC3-8267-12D19B9DA4F5}"/>
-    <hyperlink ref="K52" r:id="rId37" xr:uid="{0F2FBBA9-5A51-4F69-9755-F3438AAE10D6}"/>
-    <hyperlink ref="K57" r:id="rId38" xr:uid="{711667BA-3C30-4FE7-9826-94C9A946E1E3}"/>
-    <hyperlink ref="J48" r:id="rId39" xr:uid="{01F6FC46-9E85-462A-84A3-19ECCABC0426}"/>
-    <hyperlink ref="K43" r:id="rId40" xr:uid="{7721FC71-0048-4CE0-997A-67BD6004E684}"/>
-    <hyperlink ref="K45" r:id="rId41" xr:uid="{EB742833-2097-44BE-9C21-2DC83CF7859D}"/>
-    <hyperlink ref="J39" r:id="rId42" xr:uid="{979313BD-650F-49B8-91A4-3A95F6B0DB6C}"/>
-    <hyperlink ref="K38" r:id="rId43" xr:uid="{3BB36A31-71A0-4E57-938A-4F4BA60DB93A}"/>
-    <hyperlink ref="K7" r:id="rId44" xr:uid="{39BF4239-7AA4-42ED-B651-C0A9ABC85D36}"/>
-    <hyperlink ref="J29" r:id="rId45" xr:uid="{0046B2D3-E3BE-421B-96C2-712DFC40A195}"/>
-    <hyperlink ref="K11" r:id="rId46" xr:uid="{7A007FA7-06FA-4572-8A33-6A9EC04169B6}"/>
-    <hyperlink ref="K25" r:id="rId47" xr:uid="{A716DA10-3F64-4353-832D-5D65973EA357}"/>
-    <hyperlink ref="K26" r:id="rId48" xr:uid="{DE03A91C-86C3-46D7-A3F9-8B0F6D1C48BB}"/>
-    <hyperlink ref="K28" r:id="rId49" xr:uid="{7737FA32-A017-494D-9612-4B930F7FF9B4}"/>
-    <hyperlink ref="K29" r:id="rId50" xr:uid="{284CBC0D-E0B1-456B-B49D-3AEB25A0AC04}"/>
-    <hyperlink ref="K18" r:id="rId51" xr:uid="{E7BF36E1-0B4C-4204-AA0C-016C1194BF53}"/>
-    <hyperlink ref="K30" r:id="rId52" xr:uid="{60E6BF30-948D-4862-B9CA-C0738F854E13}"/>
-    <hyperlink ref="K40" r:id="rId53" xr:uid="{0445726A-BEF0-4202-A562-F62388E532CF}"/>
-    <hyperlink ref="K27" r:id="rId54" xr:uid="{164C9F20-1327-4609-8306-753F2FBC4930}"/>
-    <hyperlink ref="K19" r:id="rId55" xr:uid="{ECEC2631-F779-4C3E-8023-F797689B1BA7}"/>
-    <hyperlink ref="K24" r:id="rId56" xr:uid="{C2763E50-45C0-4F49-8C71-948FEFE4A5BA}"/>
-    <hyperlink ref="K33" r:id="rId57" xr:uid="{F3C17C06-C75D-4B30-9184-4C7F2AB3A3EB}"/>
-    <hyperlink ref="K34" r:id="rId58" xr:uid="{1F13BDD3-773C-4D6F-A9FF-D7368D22E426}"/>
-    <hyperlink ref="K53" r:id="rId59" xr:uid="{D0649255-1AF8-4852-8F0A-71747BBD0561}"/>
-    <hyperlink ref="K16" r:id="rId60" xr:uid="{6C681A6F-5BC3-4A2E-8803-B47814E3E649}"/>
-    <hyperlink ref="K12" r:id="rId61" xr:uid="{4D1F60AD-0F12-4248-9EDC-0342FA3A9E16}"/>
-    <hyperlink ref="K39" r:id="rId62" xr:uid="{BC8AF356-2712-4561-8768-7BDA19739073}"/>
-    <hyperlink ref="K36" r:id="rId63" xr:uid="{C17B5985-7F10-490B-89A4-E439DF52E2D3}"/>
-    <hyperlink ref="K51" r:id="rId64" xr:uid="{D600D3FF-C4CA-4323-A73D-DC6D1B8D3263}"/>
-    <hyperlink ref="K54" r:id="rId65" xr:uid="{30B3E14A-A8B0-4A72-9691-52AEC023D3AE}"/>
-    <hyperlink ref="K61" r:id="rId66" xr:uid="{DD47E6AB-3F10-4CC4-9665-5B9F4CAA251D}"/>
-    <hyperlink ref="K46" r:id="rId67" xr:uid="{F4A211EA-3FF2-4EB9-A49B-69416581C321}"/>
-    <hyperlink ref="K47" r:id="rId68" xr:uid="{986F8FEB-9DE0-4C83-9556-D21C1798D8A6}"/>
-    <hyperlink ref="K59" r:id="rId69" xr:uid="{022F3606-06A3-4750-BD88-1AC2F0D1DE52}"/>
-    <hyperlink ref="K44" r:id="rId70" xr:uid="{F980623A-7913-43A5-9A5C-0D3022386A08}"/>
-    <hyperlink ref="K48" r:id="rId71" xr:uid="{68D9F805-EC8D-4A66-A0A7-61A3F69F46AB}"/>
-    <hyperlink ref="K58" r:id="rId72" xr:uid="{4EA12311-DDCC-48D4-A6BA-4D99903BD541}"/>
-    <hyperlink ref="K50" r:id="rId73" xr:uid="{C47A4DFD-8B04-4A3A-A436-BB9C62EE48C5}"/>
-    <hyperlink ref="K60" r:id="rId74" xr:uid="{D6F34887-786B-4CDA-8BFA-F4870D073135}"/>
-    <hyperlink ref="K63" r:id="rId75" xr:uid="{2E4ED292-FC0F-41AD-A5B9-BC08DA52292D}"/>
-    <hyperlink ref="K62" r:id="rId76" xr:uid="{821D41D1-C558-4CA8-BC7B-16B6D0659D57}"/>
-    <hyperlink ref="J13" r:id="rId77" xr:uid="{9A2AC793-323E-49DC-AADB-A40B62E24402}"/>
-    <hyperlink ref="K13" r:id="rId78" xr:uid="{F7E882AD-67A4-4270-896B-E583B45947B6}"/>
-    <hyperlink ref="J20" r:id="rId79" xr:uid="{D18B1282-5727-4E67-AA19-8989266BAB08}"/>
-    <hyperlink ref="K20" r:id="rId80" xr:uid="{D5F976F5-D97D-463A-BB78-8D5E4FED278A}"/>
-    <hyperlink ref="J21" r:id="rId81" xr:uid="{5C3C1709-91B8-4BAC-AB28-C8DD467CCC4F}"/>
-    <hyperlink ref="K21" r:id="rId82" xr:uid="{6EAEAC19-9EDA-4892-951C-44E664980DCB}"/>
-    <hyperlink ref="J22" r:id="rId83" xr:uid="{0E186AEA-136D-410F-921B-761211D73F45}"/>
-    <hyperlink ref="K22" r:id="rId84" xr:uid="{474962BC-622D-4BAA-9CA6-C7456D566E8E}"/>
-    <hyperlink ref="J23" r:id="rId85" xr:uid="{109F245F-78CD-48BD-A5D6-AC7D52C505E7}"/>
-    <hyperlink ref="K23" r:id="rId86" xr:uid="{A1138993-1484-441C-B80E-4E404A8EC04D}"/>
-    <hyperlink ref="J41" r:id="rId87" xr:uid="{87F589F1-50D5-4079-A71A-6CC9D6BA86E2}"/>
-    <hyperlink ref="K41" r:id="rId88" xr:uid="{491FE978-A405-4646-8B13-99EF19506C42}"/>
-    <hyperlink ref="J42" r:id="rId89" xr:uid="{8B6679C5-F52C-4450-83EF-5B1DA246AD68}"/>
-    <hyperlink ref="K42" r:id="rId90" xr:uid="{E262CD59-EDED-4B97-99FB-AEAAB34F008F}"/>
-    <hyperlink ref="J55" r:id="rId91" xr:uid="{9E106DDF-E9B7-48B3-9F2C-A634E58FD444}"/>
-    <hyperlink ref="K55" r:id="rId92" xr:uid="{F047EC1B-3060-4740-B4A2-1E512C1A0D7D}"/>
-    <hyperlink ref="K2" r:id="rId93" xr:uid="{F375362B-C751-43CA-9C5F-2AFD54C4F480}"/>
-    <hyperlink ref="K3" r:id="rId94" xr:uid="{CE9FFB12-50DE-46BF-907C-DD55F335F93D}"/>
-    <hyperlink ref="J2" r:id="rId95" xr:uid="{B3D7A390-E204-412E-B110-EB5B15892528}"/>
-    <hyperlink ref="J3" r:id="rId96" xr:uid="{65C978E0-C035-4849-96B3-42517BA63A8C}"/>
+    <hyperlink ref="J31:J33" r:id="rId5" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{9E46802A-7C66-4114-9F0B-145434CDF86D}"/>
+    <hyperlink ref="J35:J38" r:id="rId6" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{764966E2-E14A-4E57-AF94-FC9C3C3E75EB}"/>
+    <hyperlink ref="J46" r:id="rId7" xr:uid="{1BEAF126-4AAB-4F09-A5D7-9DF756D62051}"/>
+    <hyperlink ref="J48" r:id="rId8" xr:uid="{58C7702E-D0F7-4DA3-93E3-FE80859AC198}"/>
+    <hyperlink ref="J50:J53" r:id="rId9" display="https://images.hola.com/imagenes/moda/tendencias/20231128243901/taylor-swift-estilo-evolucion-pm/1-340-207/evolucion-estilo-taylor-swift-m.jpg?tx=w_680" xr:uid="{C7A98F58-2C7B-40E0-88A4-8E96B5590279}"/>
+    <hyperlink ref="J41" r:id="rId10" xr:uid="{896DD40A-FF0E-49EA-BFF7-67BB43E791D5}"/>
+    <hyperlink ref="K38" r:id="rId11" xr:uid="{644AECA0-A45A-42BE-B259-4D5B68CC57CA}"/>
+    <hyperlink ref="J47" r:id="rId12" xr:uid="{83813776-6F4B-464C-B54A-3AC8B8505F93}"/>
+    <hyperlink ref="K8" r:id="rId13" xr:uid="{303A4440-5E60-4914-A936-17D2C2165AB4}"/>
+    <hyperlink ref="J26" r:id="rId14" xr:uid="{65FF6849-86C2-4EE7-B047-C3FC0C3A9C1E}"/>
+    <hyperlink ref="K5" r:id="rId15" xr:uid="{78EA83B8-A90E-4C38-ADF5-A381AE6620EC}"/>
+    <hyperlink ref="K4" r:id="rId16" xr:uid="{5748E202-0610-4429-B59C-C85B45D21A38}"/>
+    <hyperlink ref="K6" r:id="rId17" xr:uid="{B9C5815E-C91F-4822-A60B-26ABC9D18B7A}"/>
+    <hyperlink ref="K9" r:id="rId18" xr:uid="{585A9E42-6570-4436-82E7-0D9BEA208035}"/>
+    <hyperlink ref="K14" r:id="rId19" xr:uid="{EE4CEE3B-33D1-4373-A76F-F593B224A1B3}"/>
+    <hyperlink ref="J70" r:id="rId20" xr:uid="{8BFFACAD-FAD6-405E-B992-C4A0051C18EE}"/>
+    <hyperlink ref="K70" r:id="rId21" xr:uid="{9998AC0F-FA20-4EFC-B740-6510A5F88C01}"/>
+    <hyperlink ref="J34" r:id="rId22" xr:uid="{62EC85A5-87F0-4348-AE5C-CE2ECAC5B4FE}"/>
+    <hyperlink ref="J54" r:id="rId23" xr:uid="{4720AF8A-287A-4FDC-8E47-A448C3AC3E82}"/>
+    <hyperlink ref="K33" r:id="rId24" xr:uid="{9DE2DCDC-76C5-4F67-842D-6BDECB77345A}"/>
+    <hyperlink ref="J39" r:id="rId25" xr:uid="{2080A826-3145-4186-8445-97B7EEB1AB71}"/>
+    <hyperlink ref="J44" r:id="rId26" xr:uid="{60D8C41E-67B5-47E4-8046-A73519D62041}"/>
+    <hyperlink ref="J45" r:id="rId27" xr:uid="{417A47FF-B3E4-4A6C-B84E-7CFDD9D6229E}"/>
+    <hyperlink ref="K17" r:id="rId28" xr:uid="{DD176412-7E49-4295-96A3-1D25E4F64725}"/>
+    <hyperlink ref="K32" r:id="rId29" xr:uid="{A2D82066-C73E-4108-A5D5-27FB4BD16F6C}"/>
+    <hyperlink ref="K50" r:id="rId30" xr:uid="{7A91FC10-44E5-4A1A-8DEC-CAEC33929B0F}"/>
+    <hyperlink ref="K57" r:id="rId31" xr:uid="{6335DA8F-CF08-4974-A527-F506BDE8D0F5}"/>
+    <hyperlink ref="J14" r:id="rId32" xr:uid="{748ADAD2-77C0-4CC4-9EDC-90D46D705749}"/>
+    <hyperlink ref="K10" r:id="rId33" xr:uid="{CC624DA3-8194-4F8E-A622-C4A7BBF91D03}"/>
+    <hyperlink ref="K15" r:id="rId34" xr:uid="{FC541377-2AEA-4DA6-8E18-F7E360E14921}"/>
+    <hyperlink ref="K36" r:id="rId35" xr:uid="{7B42B139-A34D-4BC3-8267-12D19B9DA4F5}"/>
+    <hyperlink ref="K53" r:id="rId36" xr:uid="{0F2FBBA9-5A51-4F69-9755-F3438AAE10D6}"/>
+    <hyperlink ref="K58" r:id="rId37" xr:uid="{711667BA-3C30-4FE7-9826-94C9A946E1E3}"/>
+    <hyperlink ref="J49" r:id="rId38" xr:uid="{01F6FC46-9E85-462A-84A3-19ECCABC0426}"/>
+    <hyperlink ref="K44" r:id="rId39" xr:uid="{7721FC71-0048-4CE0-997A-67BD6004E684}"/>
+    <hyperlink ref="K46" r:id="rId40" xr:uid="{EB742833-2097-44BE-9C21-2DC83CF7859D}"/>
+    <hyperlink ref="J40" r:id="rId41" xr:uid="{979313BD-650F-49B8-91A4-3A95F6B0DB6C}"/>
+    <hyperlink ref="K39" r:id="rId42" xr:uid="{3BB36A31-71A0-4E57-938A-4F4BA60DB93A}"/>
+    <hyperlink ref="K7" r:id="rId43" xr:uid="{39BF4239-7AA4-42ED-B651-C0A9ABC85D36}"/>
+    <hyperlink ref="J29" r:id="rId44" xr:uid="{0046B2D3-E3BE-421B-96C2-712DFC40A195}"/>
+    <hyperlink ref="K11" r:id="rId45" xr:uid="{7A007FA7-06FA-4572-8A33-6A9EC04169B6}"/>
+    <hyperlink ref="K25" r:id="rId46" xr:uid="{A716DA10-3F64-4353-832D-5D65973EA357}"/>
+    <hyperlink ref="K26" r:id="rId47" xr:uid="{DE03A91C-86C3-46D7-A3F9-8B0F6D1C48BB}"/>
+    <hyperlink ref="K28" r:id="rId48" xr:uid="{7737FA32-A017-494D-9612-4B930F7FF9B4}"/>
+    <hyperlink ref="K29" r:id="rId49" xr:uid="{284CBC0D-E0B1-456B-B49D-3AEB25A0AC04}"/>
+    <hyperlink ref="K18" r:id="rId50" xr:uid="{E7BF36E1-0B4C-4204-AA0C-016C1194BF53}"/>
+    <hyperlink ref="K31" r:id="rId51" xr:uid="{60E6BF30-948D-4862-B9CA-C0738F854E13}"/>
+    <hyperlink ref="K41" r:id="rId52" xr:uid="{0445726A-BEF0-4202-A562-F62388E532CF}"/>
+    <hyperlink ref="K27" r:id="rId53" xr:uid="{164C9F20-1327-4609-8306-753F2FBC4930}"/>
+    <hyperlink ref="K19" r:id="rId54" xr:uid="{ECEC2631-F779-4C3E-8023-F797689B1BA7}"/>
+    <hyperlink ref="K24" r:id="rId55" xr:uid="{C2763E50-45C0-4F49-8C71-948FEFE4A5BA}"/>
+    <hyperlink ref="K34" r:id="rId56" xr:uid="{F3C17C06-C75D-4B30-9184-4C7F2AB3A3EB}"/>
+    <hyperlink ref="K35" r:id="rId57" xr:uid="{1F13BDD3-773C-4D6F-A9FF-D7368D22E426}"/>
+    <hyperlink ref="K54" r:id="rId58" xr:uid="{D0649255-1AF8-4852-8F0A-71747BBD0561}"/>
+    <hyperlink ref="K16" r:id="rId59" xr:uid="{6C681A6F-5BC3-4A2E-8803-B47814E3E649}"/>
+    <hyperlink ref="K12" r:id="rId60" xr:uid="{4D1F60AD-0F12-4248-9EDC-0342FA3A9E16}"/>
+    <hyperlink ref="K40" r:id="rId61" xr:uid="{BC8AF356-2712-4561-8768-7BDA19739073}"/>
+    <hyperlink ref="K37" r:id="rId62" xr:uid="{C17B5985-7F10-490B-89A4-E439DF52E2D3}"/>
+    <hyperlink ref="K52" r:id="rId63" xr:uid="{D600D3FF-C4CA-4323-A73D-DC6D1B8D3263}"/>
+    <hyperlink ref="K55" r:id="rId64" xr:uid="{30B3E14A-A8B0-4A72-9691-52AEC023D3AE}"/>
+    <hyperlink ref="K67" r:id="rId65" xr:uid="{DD47E6AB-3F10-4CC4-9665-5B9F4CAA251D}"/>
+    <hyperlink ref="K47" r:id="rId66" xr:uid="{F4A211EA-3FF2-4EB9-A49B-69416581C321}"/>
+    <hyperlink ref="K48" r:id="rId67" xr:uid="{986F8FEB-9DE0-4C83-9556-D21C1798D8A6}"/>
+    <hyperlink ref="K65" r:id="rId68" xr:uid="{022F3606-06A3-4750-BD88-1AC2F0D1DE52}"/>
+    <hyperlink ref="K45" r:id="rId69" xr:uid="{F980623A-7913-43A5-9A5C-0D3022386A08}"/>
+    <hyperlink ref="K49" r:id="rId70" xr:uid="{68D9F805-EC8D-4A66-A0A7-61A3F69F46AB}"/>
+    <hyperlink ref="K59" r:id="rId71" xr:uid="{4EA12311-DDCC-48D4-A6BA-4D99903BD541}"/>
+    <hyperlink ref="K51" r:id="rId72" xr:uid="{C47A4DFD-8B04-4A3A-A436-BB9C62EE48C5}"/>
+    <hyperlink ref="K66" r:id="rId73" xr:uid="{D6F34887-786B-4CDA-8BFA-F4870D073135}"/>
+    <hyperlink ref="K69" r:id="rId74" xr:uid="{2E4ED292-FC0F-41AD-A5B9-BC08DA52292D}"/>
+    <hyperlink ref="K68" r:id="rId75" xr:uid="{821D41D1-C558-4CA8-BC7B-16B6D0659D57}"/>
+    <hyperlink ref="J13" r:id="rId76" xr:uid="{9A2AC793-323E-49DC-AADB-A40B62E24402}"/>
+    <hyperlink ref="K13" r:id="rId77" xr:uid="{F7E882AD-67A4-4270-896B-E583B45947B6}"/>
+    <hyperlink ref="J20" r:id="rId78" xr:uid="{D18B1282-5727-4E67-AA19-8989266BAB08}"/>
+    <hyperlink ref="K20" r:id="rId79" xr:uid="{D5F976F5-D97D-463A-BB78-8D5E4FED278A}"/>
+    <hyperlink ref="J21" r:id="rId80" xr:uid="{5C3C1709-91B8-4BAC-AB28-C8DD467CCC4F}"/>
+    <hyperlink ref="K21" r:id="rId81" xr:uid="{6EAEAC19-9EDA-4892-951C-44E664980DCB}"/>
+    <hyperlink ref="J22" r:id="rId82" xr:uid="{0E186AEA-136D-410F-921B-761211D73F45}"/>
+    <hyperlink ref="K22" r:id="rId83" xr:uid="{474962BC-622D-4BAA-9CA6-C7456D566E8E}"/>
+    <hyperlink ref="J23" r:id="rId84" xr:uid="{109F245F-78CD-48BD-A5D6-AC7D52C505E7}"/>
+    <hyperlink ref="K23" r:id="rId85" xr:uid="{A1138993-1484-441C-B80E-4E404A8EC04D}"/>
+    <hyperlink ref="J42" r:id="rId86" xr:uid="{87F589F1-50D5-4079-A71A-6CC9D6BA86E2}"/>
+    <hyperlink ref="K42" r:id="rId87" xr:uid="{491FE978-A405-4646-8B13-99EF19506C42}"/>
+    <hyperlink ref="J43" r:id="rId88" xr:uid="{8B6679C5-F52C-4450-83EF-5B1DA246AD68}"/>
+    <hyperlink ref="K43" r:id="rId89" xr:uid="{E262CD59-EDED-4B97-99FB-AEAAB34F008F}"/>
+    <hyperlink ref="J56" r:id="rId90" xr:uid="{9E106DDF-E9B7-48B3-9F2C-A634E58FD444}"/>
+    <hyperlink ref="K56" r:id="rId91" xr:uid="{F047EC1B-3060-4740-B4A2-1E512C1A0D7D}"/>
+    <hyperlink ref="K2" r:id="rId92" xr:uid="{F375362B-C751-43CA-9C5F-2AFD54C4F480}"/>
+    <hyperlink ref="K3" r:id="rId93" xr:uid="{CE9FFB12-50DE-46BF-907C-DD55F335F93D}"/>
+    <hyperlink ref="J2" r:id="rId94" xr:uid="{B3D7A390-E204-412E-B110-EB5B15892528}"/>
+    <hyperlink ref="J3" r:id="rId95" xr:uid="{65C978E0-C035-4849-96B3-42517BA63A8C}"/>
+    <hyperlink ref="J60" r:id="rId96" xr:uid="{AF4B9B26-72A9-40CC-B944-8EB079D72BF6}"/>
+    <hyperlink ref="K60" r:id="rId97" xr:uid="{697E7BFF-17AD-4152-BEC5-2A01086523B8}"/>
+    <hyperlink ref="J61" r:id="rId98" xr:uid="{8DF4DF60-B45D-4A3E-AB88-95934B8388DE}"/>
+    <hyperlink ref="K61" r:id="rId99" xr:uid="{85AF2ADE-1A02-4146-AD7A-277B27B145D7}"/>
+    <hyperlink ref="J62" r:id="rId100" xr:uid="{3AEB8D2D-04D6-4612-B6ED-EC2F9E85C9AD}"/>
+    <hyperlink ref="J71" r:id="rId101" xr:uid="{0C019A16-A51E-4F5E-9BD0-73713E2B597D}"/>
+    <hyperlink ref="J63" r:id="rId102" xr:uid="{47AE88F9-65E9-456B-AC0E-08AAF7ABC208}"/>
+    <hyperlink ref="J73" r:id="rId103" xr:uid="{2A6D6ED5-73F6-4078-880A-D02AA9104ECD}"/>
+    <hyperlink ref="K72" r:id="rId104" xr:uid="{02E880F0-7F57-420F-972F-37F3B08B370A}"/>
+    <hyperlink ref="J72" r:id="rId105" xr:uid="{6A1F0343-ADCB-410E-9936-021CCA2E01A1}"/>
+    <hyperlink ref="K64" r:id="rId106" xr:uid="{1735CDFB-DACF-46C6-8DBC-5859CA659187}"/>
+    <hyperlink ref="J64" r:id="rId107" xr:uid="{62FAD978-2C1F-4FB1-BE8F-0EFBDA50D433}"/>
+    <hyperlink ref="K63" r:id="rId108" xr:uid="{2A22720E-A8F8-4C88-B478-255E2757A284}"/>
+    <hyperlink ref="K62" r:id="rId109" xr:uid="{08A660D9-6BD8-4DA7-9D45-A1207273B237}"/>
+    <hyperlink ref="K71" r:id="rId110" xr:uid="{49EB2BA6-06CB-498E-AB7D-D8C2EDDFDD41}"/>
+    <hyperlink ref="K73" r:id="rId111" xr:uid="{A3826779-3464-43BF-9C36-E2357E1D6BED}"/>
+    <hyperlink ref="J30" r:id="rId112" xr:uid="{3CCCE5E0-C28C-4691-8DC4-D5E15E3A6231}"/>
+    <hyperlink ref="K30" r:id="rId113" xr:uid="{DBA2DE87-FCA1-457F-8191-4EB0C352E744}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId97"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId114"/>
 </worksheet>
 </file>
</xml_diff>